<commit_message>
CAR - U6 | SP U3
</commit_message>
<xml_diff>
--- a/Seminario de Proyectos/Constructo-Investigacion.xlsx
+++ b/Seminario de Proyectos/Constructo-Investigacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/izluis/Documents/Maestria/Seminario de Proyectos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5253302-BB43-B347-AF78-6AD5C393B54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630FB634-A9E2-7C4E-93EE-AE19564B62B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="560" windowWidth="24260" windowHeight="15440" xr2:uid="{1FD9CAFA-6D95-AA4B-9E3D-D3800F87B9E3}"/>
+    <workbookView xWindow="1540" yWindow="560" windowWidth="24260" windowHeight="15440" xr2:uid="{1FD9CAFA-6D95-AA4B-9E3D-D3800F87B9E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Constructo" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Constructo de investigación</t>
   </si>
@@ -67,10 +67,40 @@
     <t>Detección temprana de enfermedades cardiovasculares</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Desarrollar un modelo predictivo basado en Machine Learning y Deep Learning para la detección temprana de enfermedades cardiovasculares en México, utilizando datos clínicos de registros electrónicos de salud</t>
+  </si>
+  <si>
+    <t>Seleccionar e implementar algoritmos de Machine Learning y Deep Learning adecuados para la predicción de enfermedades cardiovasculares, evaluando su desempeño con métricas estándar.</t>
+  </si>
+  <si>
+    <t>Analizar la interpretabilidad, precisión y viabilidad clínica de los modelos predictivos generados, con el fin de facilitar su integración en entornos médicos reales.</t>
+  </si>
+  <si>
+    <t>Recolectar, limpiar y preprocesar datos clínicos relevantes provenientes de registros electrónicos de salud, asegurando su calidad y representatividad para el análisis.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ¿Cómo puede desarrollarse un modelo predictivo basado en Machine Learning y Deep Learning para la detección temprana de enfermedades cardiovasculares en México, utilizando datos clínicos de registros electrónicos de salud?</t>
+  </si>
+  <si>
+    <t>¿Qué tipo de datos clínicos deben recolectarse, limpiarse y preprocesarse para asegurar su calidad y utilidad en el desarrollo de modelos predictivos de enfermedades cardiovasculares?</t>
+  </si>
+  <si>
+    <t>¿Qué algoritmos de Machine Learning y Deep Learning ofrecen el mejor desempeño para predecir enfermedades cardiovasculares en función de los datos clínicos disponibles?</t>
+  </si>
+  <si>
+    <t>¿Cómo se puede evaluar la interpretabilidad, precisión y viabilidad clínica de los modelos predictivos generados para facilitar su integración en entornos médicos?</t>
+  </si>
+  <si>
+    <t>Es posible desarrollar un modelo predictivo basado en Machine Learning y Deep Learning que permita la detección temprana de enfermedades cardiovasculares en México, utilizando datos clínicos provenientes de registros electrónicos de salud.</t>
+  </si>
+  <si>
+    <t>Los datos clínicos provenientes de registros electrónicos de salud pueden ser recolectados, limpiados y preprocesados de manera adecuada para garantizar su calidad y utilidad en la construcción de modelos predictivos de enfermedades cardiovasculares.</t>
+  </si>
+  <si>
+    <t>Los algoritmos de Machine Learning y Deep Learning pueden ser implementados para predecir con alta precisión la aparición de enfermedades cardiovasculares a partir de datos clínicos estructurados.</t>
+  </si>
+  <si>
+    <t>Los modelos predictivos desarrollados pueden evaluarse en términos de interpretabilidad, precisión y viabilidad clínica, lo cual permitirá su integración efectiva en entornos médicos reales.</t>
   </si>
 </sst>
 </file>
@@ -321,35 +351,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -362,33 +369,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="top" textRotation="255"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -707,168 +755,188 @@
   <dimension ref="A3:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="4.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="24" customWidth="1"/>
+    <col min="3" max="3" width="4.1640625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="24" style="24" customWidth="1"/>
+    <col min="5" max="5" width="27" style="24" customWidth="1"/>
+    <col min="6" max="6" width="27.5" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="3" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="13" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="113" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="22" t="s">
+    <row r="7" spans="1:8" ht="146" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="6" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="F7" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="153" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="17">
+        <v>1</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="136" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="19">
+        <v>2</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="9">
-        <v>1</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="13">
-        <v>2</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="8"/>
+      <c r="F9" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="3"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="118" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="9">
+      <c r="B10" s="31"/>
+      <c r="C10" s="17">
         <v>3</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="8"/>
+      <c r="D10" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="3"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="10" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
-      <c r="B12" s="25" t="s">
+    <row r="12" spans="1:8" s="8" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="28" t="s">
+      <c r="C12" s="28"/>
+      <c r="D12" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-    </row>
-    <row r="13" spans="1:8" s="19" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
-      <c r="B13" s="26" t="s">
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" s="8" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27" t="s">
+      <c r="C13" s="29"/>
+      <c r="D13" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="18"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>

</xml_diff>